<commit_message>
figures put into illustrator
</commit_message>
<xml_diff>
--- a/doc/figures/Figure4/Figure4A.xlsx
+++ b/doc/figures/Figure4/Figure4A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamklie/Desktop/lab/projects/predictMEE/doc/figures/Figure4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A834E06E-2233-794C-A5B8-A7E30E85075D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B98500DD-2946-3A42-A27D-AD38D5AB5C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15940"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Figure4A" sheetId="1" r:id="rId1"/>
@@ -897,19 +897,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.84144765125785803</v>
+        <v>0.85211805912083105</v>
       </c>
       <c r="C2">
-        <v>0.84386749166322395</v>
+        <v>0.85079087811607801</v>
       </c>
       <c r="D2">
-        <v>0.84144765187419202</v>
+        <v>0.85211805912083105</v>
       </c>
       <c r="E2">
-        <v>0.84023828432715997</v>
+        <v>0.85016626531850104</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>